<commit_message>
Added week 1 hours
8 hours, 15 to come this week ;)
</commit_message>
<xml_diff>
--- a/CS297-TimeTracking.xlsx
+++ b/CS297-TimeTracking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -398,7 +398,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -449,9 +449,12 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
       <c r="C4">
         <f>B4</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <f>D4</f>
@@ -468,7 +471,7 @@
       </c>
       <c r="C5">
         <f>B5+C4</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <f>D5+E4</f>
@@ -485,7 +488,7 @@
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C13" si="1">B6+C5</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E13" si="2">D6+E5</f>
@@ -502,7 +505,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
@@ -519,7 +522,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
@@ -536,7 +539,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
@@ -553,7 +556,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
@@ -570,7 +573,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
@@ -587,7 +590,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
@@ -604,7 +607,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
I uploaded an edited Excel sheet, I like it better personally but it can always be deleted.
</commit_message>
<xml_diff>
--- a/CS297-TimeTracking.xlsx
+++ b/CS297-TimeTracking.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nestoring\Desktop\CS297\Dversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="200" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -463,9 +463,12 @@
         <f>D4</f>
         <v>6</v>
       </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
       <c r="G4">
         <f>F4</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated hours for CJ and Nestor
</commit_message>
<xml_diff>
--- a/CS297-TimeTracking.xlsx
+++ b/CS297-TimeTracking.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nestoring\Desktop\CS297\Dversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="200" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -480,15 +480,18 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <f>SUM(D4:D5)</f>
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
       </c>
       <c r="G5">
         <f>SUM(F4:F5)</f>
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -501,11 +504,14 @@
       </c>
       <c r="E6">
         <f>SUM(D4:D6)</f>
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
       </c>
       <c r="G6">
         <f>SUM(F4:F6)</f>
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -518,11 +524,11 @@
       </c>
       <c r="E7">
         <f>SUM(D4:D7)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <f>SUM(F4:F7)</f>
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -535,11 +541,11 @@
       </c>
       <c r="E8">
         <f>SUM(D4:D8)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <f>SUM(F4:F8)</f>
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -552,11 +558,11 @@
       </c>
       <c r="E9">
         <f>SUM(D4:D9)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G9">
         <f>SUM(F4:F9)</f>
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -569,11 +575,11 @@
       </c>
       <c r="E10">
         <f>SUM(D4:D10)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <f>SUM(F4:F10)</f>
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -586,11 +592,11 @@
       </c>
       <c r="E11">
         <f>SUM(D4:D11)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G11">
         <f>SUM(F4:F11)</f>
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -603,11 +609,11 @@
       </c>
       <c r="E12">
         <f>SUM(D4:D12)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <f>SUM(F4:F12)</f>
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -620,11 +626,11 @@
       </c>
       <c r="E13">
         <f>SUM(D4:D13)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G13">
         <f>SUM(F4:F13)</f>
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added hours, add numbered tiles for clones
</commit_message>
<xml_diff>
--- a/CS297-TimeTracking.xlsx
+++ b/CS297-TimeTracking.xlsx
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DF1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="200" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -526,9 +526,12 @@
         <f>SUM(D4:D7)</f>
         <v>12</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
       <c r="G7">
         <f>SUM(F4:F7)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -545,7 +548,7 @@
       </c>
       <c r="G8">
         <f>SUM(F4:F8)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -562,7 +565,7 @@
       </c>
       <c r="G9">
         <f>SUM(F4:F9)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -579,7 +582,7 @@
       </c>
       <c r="G10">
         <f>SUM(F4:F10)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -596,7 +599,7 @@
       </c>
       <c r="G11">
         <f>SUM(F4:F11)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -613,7 +616,7 @@
       </c>
       <c r="G12">
         <f>SUM(F4:F12)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -630,7 +633,7 @@
       </c>
       <c r="G13">
         <f>SUM(F4:F13)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>